<commit_message>
se agrega comentarios para aclarar el uso de los tag NUM_NIF_LLEGADA_PARTIDA, COD_PUERTO_AEROPUERTO, COD_LOCACION_PUERTO_AEROPUERTO, NOMBRE_PUERTO_AEROPUERTO para las guias de importacion y exportacion
</commit_message>
<xml_diff>
--- a/integracionConJson_GuiaRemision/DocumentacionGuiaRemisionRemitenteJson.xlsx
+++ b/integracionConJson_GuiaRemision/DocumentacionGuiaRemisionRemitenteJson.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OscarOrlandoRosa\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workfe\apijson\integracionConJson_GuiaRemision\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC5F69F-7DCA-4DE4-B880-F6B427B01F66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A32B67E-C5AC-4AC6-8212-1C5680C7166F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="24240" windowHeight="13020" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="estructura JSON" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1794" uniqueCount="1687">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1794" uniqueCount="1688">
   <si>
     <t>TAG JSON</t>
   </si>
@@ -4965,12 +4965,6 @@
     <t>url donde se publicara los PDF personalizado de mifact (muy pronto)</t>
   </si>
   <si>
-    <t>"NUM_NIF_LLEGADA_PARTIDA":"20555700785",</t>
-  </si>
-  <si>
-    <t>Numero de ruc de la empresa proveedora portuaria, aerea</t>
-  </si>
-  <si>
     <t>CONSIGNACION</t>
   </si>
   <si>
@@ -4992,9 +4986,6 @@
     <t>nombre del puerto o aeropuerto</t>
   </si>
   <si>
-    <t>enviar si se enviar el codigo del puerto o aeropuerto</t>
-  </si>
-  <si>
     <t>solo el valor 1 para puerto maritimo y 2 para aeropuerto es opcional, pero si envias el codigo del puerto deberas enviar este tag de locacion</t>
   </si>
   <si>
@@ -5340,7 +5331,19 @@
     <t>catalogo 63 o 64</t>
   </si>
   <si>
-    <t>opcional, si no tienen el dato no enviar esta linea, pero enviar el tag NUM_NIF_LLEGADA_PARTIDA y el RUC de ese TAG tiene que estar en el DAM o DS si es una importacion, si se envia tiene que ser el codigo del catalogo 63 o 64</t>
+    <t>si envias este tag, no enviar COD_PUERTO_AEROPUERTO, COD_LOCACION_PUERTO_AEROPUERTO y NOMBRE_PUERTO_AEROPUERTO</t>
+  </si>
+  <si>
+    <t>opcional, si no tienen el dato no enviar esta linea, pero enviar el tag NUM_NIF_LLEGADA_PARTIDA y el RUC de ese TAG tiene que estar en el DAM o DS, si se envia tiene que ser el codigo del catalogo 63 o 64</t>
+  </si>
+  <si>
+    <t>enviar solo si se envia el codigo del puerto o aeropuerto (tag COD_PUERTO_AEROPUERTO)</t>
+  </si>
+  <si>
+    <t>"NUM_NIF_LLEGADA_PARTIDA":"20259171891",</t>
+  </si>
+  <si>
+    <t>Numero de RUC del tercero que se usa como almacen temporal segun DAM o DS</t>
   </si>
 </sst>
 </file>
@@ -5698,7 +5701,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255"/>
@@ -5819,25 +5822,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5861,19 +5854,26 @@
     <xf numFmtId="0" fontId="8" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -6265,8 +6265,8 @@
   <dimension ref="A1:G91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F43" sqref="F43"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -6297,16 +6297,16 @@
       <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="64" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="33" t="s">
@@ -6325,7 +6325,7 @@
       <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="66"/>
+      <c r="A4" s="64"/>
       <c r="B4" s="33" t="s">
         <v>1483</v>
       </c>
@@ -6340,7 +6340,7 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="66"/>
+      <c r="A5" s="64"/>
       <c r="B5" s="44" t="s">
         <v>1484</v>
       </c>
@@ -6355,7 +6355,7 @@
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:7" ht="30">
-      <c r="A6" s="66"/>
+      <c r="A6" s="64"/>
       <c r="B6" s="44" t="s">
         <v>1485</v>
       </c>
@@ -6372,7 +6372,7 @@
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="66"/>
+      <c r="A7" s="64"/>
       <c r="B7" s="44" t="s">
         <v>1486</v>
       </c>
@@ -6387,7 +6387,7 @@
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="66"/>
+      <c r="A8" s="64"/>
       <c r="B8" s="44" t="s">
         <v>1487</v>
       </c>
@@ -6402,7 +6402,7 @@
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="66"/>
+      <c r="A9" s="64"/>
       <c r="B9" s="33" t="s">
         <v>1488</v>
       </c>
@@ -6417,7 +6417,7 @@
       <c r="G9" s="5"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="66"/>
+      <c r="A10" s="64"/>
       <c r="B10" s="44" t="s">
         <v>1489</v>
       </c>
@@ -6434,7 +6434,7 @@
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="66"/>
+      <c r="A11" s="64"/>
       <c r="B11" s="44" t="s">
         <v>1490</v>
       </c>
@@ -6451,7 +6451,7 @@
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="66"/>
+      <c r="A12" s="64"/>
       <c r="B12" s="44" t="s">
         <v>1491</v>
       </c>
@@ -6468,7 +6468,7 @@
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="66"/>
+      <c r="A13" s="64"/>
       <c r="B13" s="44" t="s">
         <v>1492</v>
       </c>
@@ -6485,7 +6485,7 @@
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="66"/>
+      <c r="A14" s="64"/>
       <c r="B14" s="44" t="s">
         <v>1493</v>
       </c>
@@ -6504,7 +6504,7 @@
       <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="66"/>
+      <c r="A15" s="64"/>
       <c r="B15" s="44" t="s">
         <v>1494</v>
       </c>
@@ -6521,7 +6521,7 @@
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="66"/>
+      <c r="A16" s="64"/>
       <c r="B16" s="33" t="s">
         <v>1495</v>
       </c>
@@ -6538,7 +6538,7 @@
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:7">
-      <c r="A17" s="66"/>
+      <c r="A17" s="64"/>
       <c r="B17" s="33" t="s">
         <v>1496</v>
       </c>
@@ -6555,7 +6555,7 @@
       <c r="G17" s="5"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="66"/>
+      <c r="A18" s="64"/>
       <c r="B18" s="33" t="s">
         <v>1497</v>
       </c>
@@ -6572,7 +6572,7 @@
       <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="66"/>
+      <c r="A19" s="64"/>
       <c r="B19" s="44" t="s">
         <v>1498</v>
       </c>
@@ -6589,7 +6589,7 @@
       <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="66"/>
+      <c r="A20" s="64"/>
       <c r="B20" s="44" t="s">
         <v>1499</v>
       </c>
@@ -6604,7 +6604,7 @@
       <c r="G20" s="5"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="66"/>
+      <c r="A21" s="64"/>
       <c r="B21" s="34" t="s">
         <v>1500</v>
       </c>
@@ -6619,7 +6619,7 @@
       <c r="G21" s="5"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="66"/>
+      <c r="A22" s="64"/>
       <c r="B22" s="33" t="s">
         <v>1501</v>
       </c>
@@ -6634,7 +6634,7 @@
       <c r="G22" s="5"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="66"/>
+      <c r="A23" s="64"/>
       <c r="B23" s="34" t="s">
         <v>1502</v>
       </c>
@@ -6649,7 +6649,7 @@
       <c r="G23" s="5"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="66"/>
+      <c r="A24" s="64"/>
       <c r="B24" s="34" t="s">
         <v>1503</v>
       </c>
@@ -6666,7 +6666,7 @@
       <c r="G24" s="5"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="66"/>
+      <c r="A25" s="64"/>
       <c r="B25" s="34" t="s">
         <v>1504</v>
       </c>
@@ -6683,7 +6683,7 @@
       <c r="G25" s="5"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="66"/>
+      <c r="A26" s="64"/>
       <c r="B26" s="34" t="s">
         <v>1505</v>
       </c>
@@ -6700,7 +6700,7 @@
       <c r="G26" s="5"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="66"/>
+      <c r="A27" s="64"/>
       <c r="B27" s="34" t="s">
         <v>1506</v>
       </c>
@@ -6717,7 +6717,7 @@
       <c r="G27" s="5"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="66"/>
+      <c r="A28" s="64"/>
       <c r="B28" s="34" t="s">
         <v>1507</v>
       </c>
@@ -6734,7 +6734,7 @@
       <c r="G28" s="5"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="66"/>
+      <c r="A29" s="64"/>
       <c r="B29" s="34" t="s">
         <v>1508</v>
       </c>
@@ -6751,7 +6751,7 @@
       <c r="G29" s="5"/>
     </row>
     <row r="30" spans="1:7" ht="15" customHeight="1">
-      <c r="A30" s="66"/>
+      <c r="A30" s="64"/>
       <c r="B30" s="34" t="s">
         <v>1509</v>
       </c>
@@ -6762,13 +6762,13 @@
         <v>19</v>
       </c>
       <c r="E30" s="9"/>
-      <c r="F30" s="67" t="s">
+      <c r="F30" s="65" t="s">
         <v>1426</v>
       </c>
       <c r="G30" s="5"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="66"/>
+      <c r="A31" s="64"/>
       <c r="B31" s="34" t="s">
         <v>1510</v>
       </c>
@@ -6781,11 +6781,11 @@
       <c r="E31" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="F31" s="67"/>
+      <c r="F31" s="65"/>
       <c r="G31" s="5"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="66"/>
+      <c r="A32" s="64"/>
       <c r="B32" s="34" t="s">
         <v>1511</v>
       </c>
@@ -6796,11 +6796,11 @@
         <v>61</v>
       </c>
       <c r="E32" s="5"/>
-      <c r="F32" s="67"/>
+      <c r="F32" s="65"/>
       <c r="G32" s="5"/>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" s="66"/>
+      <c r="A33" s="64"/>
       <c r="B33" s="34" t="s">
         <v>1512</v>
       </c>
@@ -6817,7 +6817,7 @@
       <c r="G33" s="5"/>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" s="66"/>
+      <c r="A34" s="64"/>
       <c r="B34" s="34" t="s">
         <v>1513</v>
       </c>
@@ -6836,7 +6836,7 @@
       <c r="G34" s="5"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="66"/>
+      <c r="A35" s="64"/>
       <c r="B35" s="34" t="s">
         <v>1514</v>
       </c>
@@ -6853,7 +6853,7 @@
       <c r="G35" s="5"/>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" s="66"/>
+      <c r="A36" s="64"/>
       <c r="B36" s="34" t="s">
         <v>1397</v>
       </c>
@@ -6870,7 +6870,7 @@
       <c r="G36" s="5"/>
     </row>
     <row r="37" spans="1:7">
-      <c r="A37" s="66"/>
+      <c r="A37" s="64"/>
       <c r="B37" s="34" t="s">
         <v>1515</v>
       </c>
@@ -6887,7 +6887,7 @@
       <c r="G37" s="5"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="66"/>
+      <c r="A38" s="64"/>
       <c r="B38" s="34" t="s">
         <v>1516</v>
       </c>
@@ -6904,7 +6904,7 @@
       <c r="G38" s="5"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="66"/>
+      <c r="A39" s="64"/>
       <c r="B39" s="34" t="s">
         <v>1517</v>
       </c>
@@ -6921,7 +6921,7 @@
       <c r="G39" s="5"/>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="66"/>
+      <c r="A40" s="64"/>
       <c r="B40" s="34" t="s">
         <v>1518</v>
       </c>
@@ -6938,7 +6938,7 @@
       <c r="G40" s="5"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="66"/>
+      <c r="A41" s="64"/>
       <c r="B41" s="34" t="s">
         <v>1519</v>
       </c>
@@ -6954,147 +6954,149 @@
       </c>
       <c r="G41" s="5"/>
     </row>
-    <row r="42" spans="1:7">
-      <c r="A42" s="66"/>
+    <row r="42" spans="1:7" ht="30">
+      <c r="A42" s="64"/>
       <c r="B42" s="45" t="s">
+        <v>1686</v>
+      </c>
+      <c r="C42" s="25" t="s">
+        <v>1687</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42" s="5"/>
+      <c r="F42" s="25" t="s">
+        <v>1683</v>
+      </c>
+      <c r="G42" s="5"/>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="64"/>
+      <c r="B43" s="45" t="s">
+        <v>1562</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>1563</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E43" s="43" t="s">
+        <v>1682</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>1684</v>
+      </c>
+      <c r="G43" s="5"/>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="64"/>
+      <c r="B44" s="45" t="s">
         <v>1564</v>
       </c>
-      <c r="C42" s="6" t="s">
-        <v>1565</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E42" s="43" t="s">
-        <v>1685</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>1686</v>
-      </c>
-      <c r="G42" s="5"/>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" s="66"/>
-      <c r="B43" s="45" t="s">
+      <c r="C44" s="6" t="s">
         <v>1566</v>
       </c>
-      <c r="C43" s="6" t="s">
-        <v>1568</v>
-      </c>
-      <c r="D43" s="6" t="s">
+      <c r="D44" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="E43" s="5"/>
-      <c r="F43" s="6" t="s">
-        <v>1571</v>
-      </c>
-      <c r="G43" s="5"/>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="A44" s="66"/>
-      <c r="B44" s="45" t="s">
-        <v>1567</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>1569</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>61</v>
       </c>
       <c r="E44" s="5"/>
       <c r="F44" s="6" t="s">
-        <v>1570</v>
+        <v>1568</v>
       </c>
       <c r="G44" s="5"/>
     </row>
     <row r="45" spans="1:7">
-      <c r="A45" s="66"/>
-      <c r="B45" s="34" t="s">
-        <v>1520</v>
+      <c r="A45" s="64"/>
+      <c r="B45" s="45" t="s">
+        <v>1565</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D45" s="6"/>
+        <v>1567</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="E45" s="5"/>
       <c r="F45" s="6" t="s">
+        <v>1685</v>
+      </c>
+      <c r="G45" s="5"/>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="64"/>
+      <c r="B46" s="34" t="s">
+        <v>1520</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D46" s="6"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="G45" s="5"/>
-    </row>
-    <row r="46" spans="1:7" ht="45">
-      <c r="A46" s="66"/>
-      <c r="B46" s="34" t="s">
+      <c r="G46" s="5"/>
+    </row>
+    <row r="47" spans="1:7" ht="45">
+      <c r="A47" s="64"/>
+      <c r="B47" s="34" t="s">
         <v>1400</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C47" s="6" t="s">
         <v>1401</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E46" s="5"/>
-      <c r="F46" s="25" t="s">
-        <v>1402</v>
-      </c>
-      <c r="G46" s="5"/>
-    </row>
-    <row r="47" spans="1:7" ht="90">
-      <c r="A47" s="66"/>
-      <c r="B47" s="34" t="s">
-        <v>1403</v>
-      </c>
-      <c r="C47" s="6" t="s">
-        <v>1404</v>
       </c>
       <c r="D47" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E47" s="5"/>
       <c r="F47" s="25" t="s">
-        <v>1405</v>
+        <v>1402</v>
       </c>
       <c r="G47" s="5"/>
     </row>
-    <row r="48" spans="1:7" ht="45">
-      <c r="A48" s="1"/>
-      <c r="B48" s="44" t="s">
-        <v>1521</v>
-      </c>
-      <c r="C48" s="25" t="s">
-        <v>1406</v>
+    <row r="48" spans="1:7" ht="90">
+      <c r="A48" s="64"/>
+      <c r="B48" s="34" t="s">
+        <v>1403</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>1404</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>1407</v>
+        <v>17</v>
       </c>
       <c r="E48" s="5"/>
       <c r="F48" s="25" t="s">
-        <v>1408</v>
+        <v>1405</v>
       </c>
       <c r="G48" s="5"/>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" ht="45">
       <c r="A49" s="1"/>
       <c r="B49" s="44" t="s">
-        <v>1409</v>
+        <v>1521</v>
       </c>
       <c r="C49" s="25" t="s">
-        <v>1410</v>
+        <v>1406</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>1413</v>
+        <v>1407</v>
       </c>
       <c r="E49" s="5"/>
-      <c r="F49" s="25"/>
+      <c r="F49" s="25" t="s">
+        <v>1408</v>
+      </c>
       <c r="G49" s="5"/>
     </row>
-    <row r="50" spans="1:7" ht="30">
+    <row r="50" spans="1:7">
       <c r="A50" s="1"/>
       <c r="B50" s="44" t="s">
-        <v>1411</v>
+        <v>1409</v>
       </c>
       <c r="C50" s="25" t="s">
-        <v>1412</v>
+        <v>1410</v>
       </c>
       <c r="D50" s="6" t="s">
         <v>1413</v>
@@ -7105,11 +7107,11 @@
     </row>
     <row r="51" spans="1:7" ht="30">
       <c r="A51" s="1"/>
-      <c r="B51" s="45" t="s">
-        <v>1543</v>
+      <c r="B51" s="44" t="s">
+        <v>1411</v>
       </c>
       <c r="C51" s="25" t="s">
-        <v>1544</v>
+        <v>1412</v>
       </c>
       <c r="D51" s="6" t="s">
         <v>1413</v>
@@ -7118,59 +7120,57 @@
       <c r="F51" s="25"/>
       <c r="G51" s="5"/>
     </row>
-    <row r="52" spans="1:7" ht="45">
+    <row r="52" spans="1:7" ht="30">
       <c r="A52" s="1"/>
-      <c r="B52" s="44" t="s">
+      <c r="B52" s="45" t="s">
+        <v>1543</v>
+      </c>
+      <c r="C52" s="25" t="s">
+        <v>1544</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>1413</v>
+      </c>
+      <c r="E52" s="5"/>
+      <c r="F52" s="25"/>
+      <c r="G52" s="5"/>
+    </row>
+    <row r="53" spans="1:7" ht="45">
+      <c r="A53" s="1"/>
+      <c r="B53" s="44" t="s">
         <v>1415</v>
       </c>
-      <c r="C52" s="25" t="s">
+      <c r="C53" s="25" t="s">
         <v>1416</v>
       </c>
-      <c r="D52" s="6" t="s">
+      <c r="D53" s="6" t="s">
         <v>1424</v>
-      </c>
-      <c r="E52" s="5"/>
-      <c r="F52" s="25" t="s">
-        <v>1417</v>
-      </c>
-      <c r="G52" s="5"/>
-    </row>
-    <row r="53" spans="1:7" ht="30">
-      <c r="A53" s="1"/>
-      <c r="B53" s="45" t="s">
-        <v>1460</v>
-      </c>
-      <c r="C53" s="25" t="s">
-        <v>1461</v>
-      </c>
-      <c r="D53" s="6" t="s">
-        <v>17</v>
       </c>
       <c r="E53" s="5"/>
       <c r="F53" s="25" t="s">
-        <v>1473</v>
+        <v>1417</v>
       </c>
       <c r="G53" s="5"/>
     </row>
-    <row r="54" spans="1:7">
-      <c r="A54" s="58"/>
+    <row r="54" spans="1:7" ht="30">
+      <c r="A54" s="1"/>
       <c r="B54" s="45" t="s">
-        <v>1561</v>
+        <v>1460</v>
       </c>
       <c r="C54" s="25" t="s">
-        <v>1562</v>
+        <v>1461</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E54" s="5"/>
       <c r="F54" s="25" t="s">
-        <v>1562</v>
+        <v>1473</v>
       </c>
       <c r="G54" s="5"/>
     </row>
     <row r="55" spans="1:7" ht="15" customHeight="1">
-      <c r="A55" s="69" t="s">
+      <c r="A55" s="67" t="s">
         <v>1418</v>
       </c>
       <c r="B55" s="36" t="s">
@@ -7187,7 +7187,7 @@
       <c r="G55" s="5"/>
     </row>
     <row r="56" spans="1:7" ht="28.5" customHeight="1">
-      <c r="A56" s="70"/>
+      <c r="A56" s="68"/>
       <c r="B56" s="36" t="s">
         <v>1474</v>
       </c>
@@ -7202,7 +7202,7 @@
       <c r="G56" s="5"/>
     </row>
     <row r="57" spans="1:7">
-      <c r="A57" s="70"/>
+      <c r="A57" s="68"/>
       <c r="B57" s="36" t="s">
         <v>1476</v>
       </c>
@@ -7217,7 +7217,7 @@
       <c r="G57" s="5"/>
     </row>
     <row r="58" spans="1:7">
-      <c r="A58" s="70"/>
+      <c r="A58" s="68"/>
       <c r="B58" s="36" t="s">
         <v>1477</v>
       </c>
@@ -7232,7 +7232,7 @@
       <c r="G58" s="5"/>
     </row>
     <row r="59" spans="1:7">
-      <c r="A59" s="70"/>
+      <c r="A59" s="68"/>
       <c r="B59" s="36" t="s">
         <v>1478</v>
       </c>
@@ -7249,7 +7249,7 @@
       <c r="G59" s="37"/>
     </row>
     <row r="60" spans="1:7">
-      <c r="A60" s="70"/>
+      <c r="A60" s="68"/>
       <c r="B60" s="36" t="s">
         <v>1479</v>
       </c>
@@ -7268,7 +7268,7 @@
       <c r="G60" s="37"/>
     </row>
     <row r="61" spans="1:7" ht="60">
-      <c r="A61" s="70"/>
+      <c r="A61" s="68"/>
       <c r="B61" s="51" t="s">
         <v>1466</v>
       </c>
@@ -7286,7 +7286,7 @@
       </c>
     </row>
     <row r="62" spans="1:7">
-      <c r="A62" s="70"/>
+      <c r="A62" s="68"/>
       <c r="B62" s="51" t="s">
         <v>1465</v>
       </c>
@@ -7302,7 +7302,7 @@
       </c>
     </row>
     <row r="63" spans="1:7">
-      <c r="A63" s="71"/>
+      <c r="A63" s="69"/>
       <c r="B63" s="51" t="s">
         <v>1469</v>
       </c>
@@ -7320,7 +7320,7 @@
       </c>
     </row>
     <row r="64" spans="1:7">
-      <c r="A64" s="68" t="s">
+      <c r="A64" s="66" t="s">
         <v>1421</v>
       </c>
       <c r="B64" s="40" t="s">
@@ -7338,7 +7338,7 @@
       <c r="F64" s="5"/>
     </row>
     <row r="65" spans="1:6" ht="60">
-      <c r="A65" s="68"/>
+      <c r="A65" s="66"/>
       <c r="B65" s="38" t="s">
         <v>1420</v>
       </c>
@@ -7354,7 +7354,7 @@
       </c>
     </row>
     <row r="66" spans="1:6">
-      <c r="A66" s="68"/>
+      <c r="A66" s="66"/>
       <c r="B66" s="41"/>
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
@@ -7362,7 +7362,7 @@
       <c r="F66" s="5"/>
     </row>
     <row r="67" spans="1:6">
-      <c r="A67" s="68"/>
+      <c r="A67" s="66"/>
       <c r="B67" s="39"/>
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
@@ -7370,10 +7370,10 @@
       <c r="F67" s="5"/>
     </row>
     <row r="69" spans="1:6">
-      <c r="B69" s="60" t="s">
+      <c r="B69" s="70" t="s">
         <v>1548</v>
       </c>
-      <c r="C69" s="60"/>
+      <c r="C69" s="70"/>
     </row>
     <row r="70" spans="1:6">
       <c r="B70" s="54" t="s">
@@ -7398,10 +7398,10 @@
       </c>
     </row>
     <row r="73" spans="1:6">
-      <c r="B73" s="60" t="s">
+      <c r="B73" s="70" t="s">
         <v>1554</v>
       </c>
-      <c r="C73" s="60"/>
+      <c r="C73" s="70"/>
     </row>
     <row r="74" spans="1:6">
       <c r="B74" s="5" t="s">
@@ -7441,74 +7441,74 @@
       </c>
     </row>
     <row r="80" spans="1:6" ht="26.25" customHeight="1">
-      <c r="B80" s="61" t="s">
+      <c r="B80" s="71" t="s">
         <v>1556</v>
       </c>
-      <c r="C80" s="61"/>
+      <c r="C80" s="71"/>
     </row>
     <row r="81" spans="2:3">
-      <c r="B81" s="61"/>
-      <c r="C81" s="61"/>
+      <c r="B81" s="71"/>
+      <c r="C81" s="71"/>
     </row>
     <row r="82" spans="2:3">
-      <c r="B82" s="61"/>
-      <c r="C82" s="61"/>
+      <c r="B82" s="71"/>
+      <c r="C82" s="71"/>
     </row>
     <row r="83" spans="2:3">
-      <c r="B83" s="61"/>
-      <c r="C83" s="61"/>
+      <c r="B83" s="71"/>
+      <c r="C83" s="71"/>
     </row>
     <row r="84" spans="2:3">
-      <c r="B84" s="63" t="s">
+      <c r="B84" s="73" t="s">
         <v>1557</v>
       </c>
-      <c r="C84" s="64"/>
+      <c r="C84" s="74"/>
     </row>
     <row r="85" spans="2:3">
-      <c r="B85" s="62" t="s">
+      <c r="B85" s="72" t="s">
         <v>1558</v>
       </c>
-      <c r="C85" s="62"/>
+      <c r="C85" s="72"/>
     </row>
     <row r="86" spans="2:3">
-      <c r="B86" s="62"/>
-      <c r="C86" s="62"/>
+      <c r="B86" s="72"/>
+      <c r="C86" s="72"/>
     </row>
     <row r="87" spans="2:3">
-      <c r="B87" s="62"/>
-      <c r="C87" s="62"/>
+      <c r="B87" s="72"/>
+      <c r="C87" s="72"/>
     </row>
     <row r="88" spans="2:3">
-      <c r="B88" s="62"/>
-      <c r="C88" s="62"/>
+      <c r="B88" s="72"/>
+      <c r="C88" s="72"/>
     </row>
     <row r="89" spans="2:3">
-      <c r="B89" s="62" t="s">
+      <c r="B89" s="72" t="s">
         <v>1559</v>
       </c>
-      <c r="C89" s="62"/>
+      <c r="C89" s="72"/>
     </row>
     <row r="90" spans="2:3">
-      <c r="B90" s="62"/>
-      <c r="C90" s="62"/>
+      <c r="B90" s="72"/>
+      <c r="C90" s="72"/>
     </row>
     <row r="91" spans="2:3">
-      <c r="B91" s="62"/>
-      <c r="C91" s="62"/>
+      <c r="B91" s="72"/>
+      <c r="C91" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="A3:A47"/>
-    <mergeCell ref="F30:F32"/>
-    <mergeCell ref="A64:A67"/>
-    <mergeCell ref="A55:A63"/>
     <mergeCell ref="B69:C69"/>
     <mergeCell ref="B73:C73"/>
     <mergeCell ref="B80:C83"/>
     <mergeCell ref="B85:C88"/>
     <mergeCell ref="B89:C91"/>
     <mergeCell ref="B84:C84"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="A3:A48"/>
+    <mergeCell ref="F30:F32"/>
+    <mergeCell ref="A64:A67"/>
+    <mergeCell ref="A55:A63"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E13" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -7524,7 +7524,7 @@
     <hyperlink ref="E64" location="'Catalogo 01'!A1" display="catalogo 01" xr:uid="{9050861D-93B0-41E8-802D-61BA1AF7918E}"/>
     <hyperlink ref="E61" r:id="rId4" xr:uid="{488731D0-1683-4F77-A777-5332465915AF}"/>
     <hyperlink ref="E63" location="'Catalogo 62'!A1" display="'Catalogo 62'!A1" xr:uid="{7B431874-ABA0-4BA2-96C0-01742BA265F1}"/>
-    <hyperlink ref="E42" location="'Catalogo 63 y 64'!A1" display="catalogo 63 o 64" xr:uid="{923DF33F-7098-437C-BBF5-DBAAE3F22788}"/>
+    <hyperlink ref="E43" location="'Catalogo 63 y 64'!A1" display="catalogo 63 o 64" xr:uid="{923DF33F-7098-437C-BBF5-DBAAE3F22788}"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555496" right="0.69930555555555496" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
@@ -7945,11 +7945,11 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="58" t="s">
         <v>152</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -8201,22 +8201,22 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="75" t="s">
         <v>1525</v>
       </c>
       <c r="B3" s="49" t="s">
         <v>1526</v>
       </c>
-      <c r="C3" s="73" t="s">
+      <c r="C3" s="76" t="s">
         <v>1527</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="72"/>
+      <c r="A4" s="75"/>
       <c r="B4" s="49" t="s">
         <v>1525</v>
       </c>
-      <c r="C4" s="73"/>
+      <c r="C4" s="76"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="30">
@@ -8393,12 +8393,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="26.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="46" t="s">
         <v>1523</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>1572</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -8409,15 +8409,15 @@
         <v>1430</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>1573</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="30" t="s">
-        <v>1574</v>
+        <v>1571</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>1575</v>
+        <v>1572</v>
       </c>
       <c r="C4" s="30">
         <v>200801</v>
@@ -8425,21 +8425,21 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="30" t="s">
-        <v>1576</v>
+        <v>1573</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>1577</v>
+        <v>1574</v>
       </c>
       <c r="C5" s="30" t="s">
-        <v>1578</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="30" t="s">
-        <v>1579</v>
+        <v>1576</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>1580</v>
+        <v>1577</v>
       </c>
       <c r="C6" s="30">
         <v>150119</v>
@@ -8447,10 +8447,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="30" t="s">
-        <v>1581</v>
+        <v>1578</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>1582</v>
+        <v>1579</v>
       </c>
       <c r="C7" s="30">
         <v>150605</v>
@@ -8458,21 +8458,21 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="30" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>1584</v>
+        <v>1581</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>1585</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="30" t="s">
-        <v>1586</v>
+        <v>1583</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>1587</v>
+        <v>1584</v>
       </c>
       <c r="C9" s="30">
         <v>140113</v>
@@ -8480,10 +8480,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="30" t="s">
-        <v>1588</v>
+        <v>1585</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>1589</v>
+        <v>1586</v>
       </c>
       <c r="C10" s="30">
         <v>150801</v>
@@ -8491,21 +8491,21 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="30" t="s">
-        <v>1590</v>
+        <v>1587</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>1591</v>
+        <v>1588</v>
       </c>
       <c r="C11" s="30" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="30" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>1594</v>
+        <v>1591</v>
       </c>
       <c r="C12" s="30">
         <v>180301</v>
@@ -8513,10 +8513,10 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="30" t="s">
-        <v>1595</v>
+        <v>1592</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>1596</v>
+        <v>1593</v>
       </c>
       <c r="C13" s="30">
         <v>160101</v>
@@ -8524,21 +8524,21 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="30" t="s">
-        <v>1597</v>
+        <v>1594</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>1598</v>
+        <v>1595</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>1599</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="30" t="s">
-        <v>1600</v>
+        <v>1597</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>1601</v>
+        <v>1598</v>
       </c>
       <c r="C15" s="30">
         <v>200501</v>
@@ -8546,10 +8546,10 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="30" t="s">
-        <v>1602</v>
+        <v>1599</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>1603</v>
+        <v>1600</v>
       </c>
       <c r="C16" s="30">
         <v>110505</v>
@@ -8557,10 +8557,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="30" t="s">
-        <v>1604</v>
+        <v>1601</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>1605</v>
+        <v>1602</v>
       </c>
       <c r="C17" s="30">
         <v>250101</v>
@@ -8568,10 +8568,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="30" t="s">
-        <v>1606</v>
+        <v>1603</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>1607</v>
+        <v>1604</v>
       </c>
       <c r="C18" s="30">
         <v>210101</v>
@@ -8579,10 +8579,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="30" t="s">
-        <v>1608</v>
+        <v>1605</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>1609</v>
+        <v>1606</v>
       </c>
       <c r="C19" s="30">
         <v>130109</v>
@@ -8590,10 +8590,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="30" t="s">
-        <v>1610</v>
+        <v>1607</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>1611</v>
+        <v>1608</v>
       </c>
       <c r="C20" s="30">
         <v>110304</v>
@@ -8601,10 +8601,10 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="30" t="s">
-        <v>1612</v>
+        <v>1609</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>1613</v>
+        <v>1610</v>
       </c>
       <c r="C21" s="30">
         <v>150204</v>
@@ -8612,10 +8612,10 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="30" t="s">
-        <v>1614</v>
+        <v>1611</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>1615</v>
+        <v>1612</v>
       </c>
       <c r="C22" s="30">
         <v>200701</v>
@@ -8623,10 +8623,10 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="30" t="s">
-        <v>1616</v>
+        <v>1613</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>1617</v>
+        <v>1614</v>
       </c>
       <c r="C23" s="30">
         <v>160201</v>
@@ -8634,19 +8634,19 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="30" t="s">
-        <v>1618</v>
+        <v>1615</v>
       </c>
       <c r="B24" s="31" t="s">
-        <v>1619</v>
+        <v>1616</v>
       </c>
       <c r="C24" s="30">
         <v>240103</v>
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="74"/>
-      <c r="B25" s="75"/>
-      <c r="C25" s="76"/>
+      <c r="A25" s="59"/>
+      <c r="B25" s="60"/>
+      <c r="C25" s="61"/>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="46" t="s">
@@ -8656,12 +8656,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="26.25">
+    <row r="28" spans="1:3">
       <c r="A28" s="46" t="s">
         <v>1523</v>
       </c>
       <c r="B28" s="48" t="s">
-        <v>1620</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -8672,103 +8672,103 @@
         <v>1430</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>1573</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="30" t="s">
-        <v>1621</v>
+        <v>1618</v>
       </c>
       <c r="B30" s="31" t="s">
-        <v>1622</v>
+        <v>1619</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>1623</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="30" t="s">
-        <v>1624</v>
+        <v>1621</v>
       </c>
       <c r="B31" s="31" t="s">
-        <v>1625</v>
+        <v>1622</v>
       </c>
       <c r="C31" s="30" t="s">
-        <v>1626</v>
+        <v>1623</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="30" t="s">
-        <v>1627</v>
+        <v>1624</v>
       </c>
       <c r="B32" s="31" t="s">
-        <v>1628</v>
+        <v>1625</v>
       </c>
       <c r="C32" s="30" t="s">
-        <v>1629</v>
+        <v>1626</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="30" t="s">
-        <v>1630</v>
+        <v>1627</v>
       </c>
       <c r="B33" s="31" t="s">
-        <v>1631</v>
+        <v>1628</v>
       </c>
       <c r="C33" s="30" t="s">
-        <v>1632</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="30" t="s">
-        <v>1633</v>
+        <v>1630</v>
       </c>
       <c r="B34" s="31" t="s">
-        <v>1634</v>
+        <v>1631</v>
       </c>
       <c r="C34" s="30" t="s">
-        <v>1635</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="30" t="s">
-        <v>1583</v>
+        <v>1580</v>
       </c>
       <c r="B35" s="31" t="s">
-        <v>1636</v>
+        <v>1633</v>
       </c>
       <c r="C35" s="30" t="s">
-        <v>1637</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="30" t="s">
-        <v>1638</v>
+        <v>1635</v>
       </c>
       <c r="B36" s="31" t="s">
-        <v>1639</v>
+        <v>1636</v>
       </c>
       <c r="C36" s="30" t="s">
-        <v>1640</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" s="30" t="s">
-        <v>1641</v>
+        <v>1638</v>
       </c>
       <c r="B37" s="31" t="s">
-        <v>1642</v>
+        <v>1639</v>
       </c>
       <c r="C37" s="30" t="s">
-        <v>1643</v>
+        <v>1640</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="30" t="s">
-        <v>1644</v>
+        <v>1641</v>
       </c>
       <c r="B38" s="31" t="s">
-        <v>1645</v>
+        <v>1642</v>
       </c>
       <c r="C38" s="30">
         <v>140101</v>
@@ -8776,10 +8776,10 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="30" t="s">
-        <v>1646</v>
+        <v>1643</v>
       </c>
       <c r="B39" s="31" t="s">
-        <v>1647</v>
+        <v>1644</v>
       </c>
       <c r="C39" s="30">
         <v>100101</v>
@@ -8787,10 +8787,10 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="30" t="s">
-        <v>1648</v>
+        <v>1645</v>
       </c>
       <c r="B40" s="31" t="s">
-        <v>1594</v>
+        <v>1591</v>
       </c>
       <c r="C40" s="30">
         <v>180301</v>
@@ -8798,10 +8798,10 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="30" t="s">
-        <v>1595</v>
-      </c>
-      <c r="B41" s="77" t="s">
-        <v>1649</v>
+        <v>1592</v>
+      </c>
+      <c r="B41" s="62" t="s">
+        <v>1646</v>
       </c>
       <c r="C41" s="30">
         <v>160101</v>
@@ -8809,21 +8809,21 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="30" t="s">
-        <v>1650</v>
+        <v>1647</v>
       </c>
       <c r="B42" s="31" t="s">
-        <v>1651</v>
+        <v>1648</v>
       </c>
       <c r="C42" s="30" t="s">
-        <v>1652</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="30" t="s">
-        <v>1653</v>
+        <v>1650</v>
       </c>
       <c r="B43" s="31" t="s">
-        <v>1654</v>
+        <v>1651</v>
       </c>
       <c r="C43" s="30">
         <v>220601</v>
@@ -8831,10 +8831,10 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="30" t="s">
-        <v>1655</v>
+        <v>1652</v>
       </c>
       <c r="B44" s="31" t="s">
-        <v>1656</v>
+        <v>1653</v>
       </c>
       <c r="C44" s="30">
         <v>211101</v>
@@ -8842,10 +8842,10 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="30" t="s">
-        <v>1657</v>
+        <v>1654</v>
       </c>
       <c r="B45" s="31" t="s">
-        <v>1658</v>
+        <v>1655</v>
       </c>
       <c r="C45" s="30">
         <v>120430</v>
@@ -8853,21 +8853,21 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="30" t="s">
-        <v>1659</v>
+        <v>1656</v>
       </c>
       <c r="B46" s="31" t="s">
-        <v>1660</v>
+        <v>1657</v>
       </c>
       <c r="C46" s="30" t="s">
-        <v>1578</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="30" t="s">
-        <v>1661</v>
+        <v>1658</v>
       </c>
       <c r="B47" s="31" t="s">
-        <v>1662</v>
+        <v>1659</v>
       </c>
       <c r="C47" s="30">
         <v>220101</v>
@@ -8875,10 +8875,10 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="30" t="s">
-        <v>1602</v>
+        <v>1599</v>
       </c>
       <c r="B48" s="31" t="s">
-        <v>1663</v>
+        <v>1660</v>
       </c>
       <c r="C48" s="30">
         <v>110506</v>
@@ -8886,10 +8886,10 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="30" t="s">
-        <v>1664</v>
+        <v>1661</v>
       </c>
       <c r="B49" s="31" t="s">
-        <v>1665</v>
+        <v>1662</v>
       </c>
       <c r="C49" s="30">
         <v>200104</v>
@@ -8897,10 +8897,10 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="30" t="s">
-        <v>1604</v>
+        <v>1601</v>
       </c>
       <c r="B50" s="31" t="s">
-        <v>1666</v>
+        <v>1663</v>
       </c>
       <c r="C50" s="30">
         <v>250105</v>
@@ -8908,10 +8908,10 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="30" t="s">
-        <v>1667</v>
+        <v>1664</v>
       </c>
       <c r="B51" s="31" t="s">
-        <v>1668</v>
+        <v>1665</v>
       </c>
       <c r="C51" s="30">
         <v>170101</v>
@@ -8919,10 +8919,10 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="30" t="s">
-        <v>1669</v>
+        <v>1666</v>
       </c>
       <c r="B52" s="31" t="s">
-        <v>1670</v>
+        <v>1667</v>
       </c>
       <c r="C52" s="30">
         <v>220801</v>
@@ -8930,10 +8930,10 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="30" t="s">
-        <v>1671</v>
+        <v>1668</v>
       </c>
       <c r="B53" s="31" t="s">
-        <v>1672</v>
+        <v>1669</v>
       </c>
       <c r="C53" s="30">
         <v>230101</v>
@@ -8941,10 +8941,10 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="30" t="s">
-        <v>1614</v>
+        <v>1611</v>
       </c>
       <c r="B54" s="31" t="s">
-        <v>1673</v>
+        <v>1670</v>
       </c>
       <c r="C54" s="30">
         <v>200701</v>
@@ -8952,10 +8952,10 @@
     </row>
     <row r="55" spans="1:3">
       <c r="A55" s="30" t="s">
-        <v>1674</v>
+        <v>1671</v>
       </c>
       <c r="B55" s="31" t="s">
-        <v>1675</v>
+        <v>1672</v>
       </c>
       <c r="C55" s="30">
         <v>220901</v>
@@ -8963,10 +8963,10 @@
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="30" t="s">
-        <v>1676</v>
+        <v>1673</v>
       </c>
       <c r="B56" s="31" t="s">
-        <v>1677</v>
+        <v>1674</v>
       </c>
       <c r="C56" s="30">
         <v>100601</v>
@@ -8974,10 +8974,10 @@
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="30" t="s">
-        <v>1678</v>
+        <v>1675</v>
       </c>
       <c r="B57" s="31" t="s">
-        <v>1679</v>
+        <v>1676</v>
       </c>
       <c r="C57" s="30">
         <v>130104</v>
@@ -8985,10 +8985,10 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="30" t="s">
-        <v>1680</v>
+        <v>1677</v>
       </c>
       <c r="B58" s="31" t="s">
-        <v>1681</v>
+        <v>1678</v>
       </c>
       <c r="C58" s="30">
         <v>240101</v>
@@ -8996,10 +8996,10 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="30" t="s">
-        <v>1682</v>
+        <v>1679</v>
       </c>
       <c r="B59" s="31" t="s">
-        <v>1683</v>
+        <v>1680</v>
       </c>
       <c r="C59" s="30">
         <v>250201</v>
@@ -9007,10 +9007,10 @@
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="30" t="s">
-        <v>1616</v>
+        <v>1613</v>
       </c>
       <c r="B60" s="31" t="s">
-        <v>1684</v>
+        <v>1681</v>
       </c>
       <c r="C60" s="30">
         <v>160201</v>

</xml_diff>